<commit_message>
Backup before adding scale to pane class
</commit_message>
<xml_diff>
--- a/Hero Class Ideas.xlsx
+++ b/Hero Class Ideas.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\OneDrive\Documents\GitHub\Dungeon_Crawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524FAF26-FF28-41C0-AF0F-5FA7C30B7133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DDBFCE-403D-405C-8EFC-5698DB5EEECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12549" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10954" yWindow="0" windowWidth="10989" windowHeight="12343" xr2:uid="{781B20D6-5C27-48E4-8F07-61E740B0FE5B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Class Roles" sheetId="1" r:id="rId1"/>
+    <sheet name="Combat Skills" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Beastmaster</t>
   </si>
@@ -135,32 +136,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Warrior</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Toughness</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Rogue</t>
     </r>
     <r>
@@ -179,15 +154,8 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Support</t>
+      <t xml:space="preserve">ROGUE
+</t>
     </r>
     <r>
       <rPr>
@@ -199,21 +167,39 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Agility</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Caster"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">
-Personality</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Caster"</t>
+Intellect</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CASTER
+</t>
     </r>
     <r>
       <rPr>
@@ -225,8 +211,39 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Intellect</t>
+    </r>
+  </si>
+  <si>
+    <t>combat_skill</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Warrior</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">
-Mind</t>
+Might</t>
     </r>
   </si>
   <si>
@@ -244,26 +261,47 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Toughness</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ROGUE
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Agility</t>
-    </r>
+      <t>Might</t>
+    </r>
+  </si>
+  <si>
+    <t>might</t>
+  </si>
+  <si>
+    <t>taunt</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>"focus enemy attack on self"</t>
+  </si>
+  <si>
+    <t>rogue</t>
+  </si>
+  <si>
+    <t>hamstring</t>
+  </si>
+  <si>
+    <t>"lowers enemy evasion and initiative (agility)"</t>
+  </si>
+  <si>
+    <t>agility</t>
+  </si>
+  <si>
+    <t>soldier</t>
+  </si>
+  <si>
+    <t>charisma</t>
+  </si>
+  <si>
+    <t>support</t>
+  </si>
+  <si>
+    <t>intellect</t>
+  </si>
+  <si>
+    <t>mage</t>
   </si>
   <si>
     <r>
@@ -280,26 +318,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Personality</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CASTER
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mind</t>
-    </r>
+      <t>Charisma</t>
+    </r>
+  </si>
+  <si>
+    <t>Support
+Charisma</t>
   </si>
 </sst>
 </file>
@@ -398,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -415,6 +439,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -422,6 +447,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -704,10 +732,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="61.3" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -718,12 +747,12 @@
     <row r="1" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -731,28 +760,28 @@
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -766,15 +795,15 @@
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -788,15 +817,15 @@
       <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -810,15 +839,15 @@
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -832,10 +861,10 @@
       <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -849,4 +878,83 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F5184F-964B-44CE-8A3D-E9399C3B33BB}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Backup before dynamic panes pt1
</commit_message>
<xml_diff>
--- a/Hero Class Ideas.xlsx
+++ b/Hero Class Ideas.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\OneDrive\Documents\GitHub\Dungeon_Crawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DDBFCE-403D-405C-8EFC-5698DB5EEECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD184F75-9A71-4F6E-B8FC-62E92F8E2D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10954" yWindow="0" windowWidth="10989" windowHeight="12343" xr2:uid="{781B20D6-5C27-48E4-8F07-61E740B0FE5B}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12549" xr2:uid="{781B20D6-5C27-48E4-8F07-61E740B0FE5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Class Roles" sheetId="1" r:id="rId1"/>
     <sheet name="Combat Skills" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>Beastmaster</t>
   </si>
@@ -325,12 +326,39 @@
     <t>Support
 Charisma</t>
   </si>
+  <si>
+    <t>Aberration</t>
+  </si>
+  <si>
+    <t>Beast</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Vermin</t>
+  </si>
+  <si>
+    <t>Corpse</t>
+  </si>
+  <si>
+    <t>Skeleton</t>
+  </si>
+  <si>
+    <t>Specter</t>
+  </si>
+  <si>
+    <t>Mortal</t>
+  </si>
+  <si>
+    <t>Mythical</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,13 +400,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -422,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -440,6 +499,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -447,9 +527,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -733,10 +810,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="67" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="61.3" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -744,19 +821,19 @@
     <col min="1" max="16384" width="11.3828125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
@@ -765,19 +842,47 @@
       <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>45</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
+      <c r="H2" s="16"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -795,13 +900,29 @@
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7"/>
+      <c r="H3" s="15"/>
+      <c r="M3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="13">
+        <v>1</v>
+      </c>
+      <c r="O3" s="9">
+        <v>2</v>
+      </c>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+    </row>
+    <row r="4" spans="1:22" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="14"/>
       <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
@@ -817,13 +938,31 @@
       <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7"/>
+      <c r="H4" s="15"/>
+      <c r="M4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="13">
+        <v>3</v>
+      </c>
+      <c r="O4" s="9">
+        <v>4</v>
+      </c>
+      <c r="P4" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+    </row>
+    <row r="5" spans="1:22" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="14"/>
       <c r="B5" s="5" t="s">
         <v>44</v>
       </c>
@@ -839,13 +978,33 @@
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="7"/>
+      <c r="H5" s="15"/>
+      <c r="M5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="13">
+        <v>6</v>
+      </c>
+      <c r="O5" s="9">
+        <v>7</v>
+      </c>
+      <c r="P5" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>9</v>
+      </c>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+    </row>
+    <row r="6" spans="1:22" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="14"/>
       <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
@@ -861,10 +1020,139 @@
       <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="8"/>
+      <c r="H6" s="15"/>
+      <c r="M6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="13">
+        <v>10</v>
+      </c>
+      <c r="O6" s="9">
+        <v>11</v>
+      </c>
+      <c r="P6" s="9">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>13</v>
+      </c>
+      <c r="R6" s="9">
+        <v>14</v>
+      </c>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+    </row>
+    <row r="7" spans="1:22" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="13">
+        <v>15</v>
+      </c>
+      <c r="O7" s="13">
+        <v>16</v>
+      </c>
+      <c r="P7" s="13">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="13">
+        <v>18</v>
+      </c>
+      <c r="R7" s="13">
+        <v>19</v>
+      </c>
+      <c r="S7" s="13">
+        <v>20</v>
+      </c>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+    </row>
+    <row r="8" spans="1:22" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N8" s="11">
+        <v>1</v>
+      </c>
+      <c r="O8" s="11">
+        <v>2</v>
+      </c>
+      <c r="P8" s="11">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>4</v>
+      </c>
+      <c r="R8" s="11">
+        <v>5</v>
+      </c>
+      <c r="S8" s="12"/>
+      <c r="T8" s="11">
+        <v>6</v>
+      </c>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+    </row>
+    <row r="9" spans="1:22" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="11">
+        <v>7</v>
+      </c>
+      <c r="O9" s="11">
+        <v>8</v>
+      </c>
+      <c r="P9" s="11">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>10</v>
+      </c>
+      <c r="R9" s="11">
+        <v>11</v>
+      </c>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="11">
+        <v>12</v>
+      </c>
+      <c r="V9" s="10"/>
+    </row>
+    <row r="10" spans="1:22" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="11">
+        <v>13</v>
+      </c>
+      <c r="O10" s="11">
+        <v>14</v>
+      </c>
+      <c r="P10" s="11">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>16</v>
+      </c>
+      <c r="R10" s="11">
+        <v>17</v>
+      </c>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="61.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>